<commit_message>
Species code updates 2020
Cleaning bits after discussing with survey team
</commit_message>
<xml_diff>
--- a/background/Species codes.xlsx
+++ b/background/Species codes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18165" yWindow="0" windowWidth="19200" windowHeight="8145"/>
+    <workbookView xWindow="19570" yWindow="0" windowWidth="19200" windowHeight="8150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="348">
   <si>
     <t>unknown</t>
   </si>
@@ -1153,6 +1153,18 @@
   </si>
   <si>
     <t>OLRIR</t>
+  </si>
+  <si>
+    <t>MEAL3</t>
+  </si>
+  <si>
+    <t>Melilotus altissimus</t>
+  </si>
+  <si>
+    <t>DEPI</t>
+  </si>
+  <si>
+    <t>Descurainia pinnata</t>
   </si>
 </sst>
 </file>
@@ -1527,20 +1539,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K238"/>
+  <dimension ref="A1:K240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>91</v>
       </c>
@@ -1560,7 +1572,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>323</v>
       </c>
@@ -1576,7 +1588,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1590,7 +1602,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -1604,7 +1616,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1632,7 +1644,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1646,7 +1658,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1660,7 +1672,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>197</v>
       </c>
@@ -1674,7 +1686,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>135</v>
       </c>
@@ -1688,7 +1700,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>86</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>200</v>
       </c>
@@ -1716,7 +1728,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1730,7 +1742,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1744,7 +1756,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>80</v>
       </c>
@@ -1758,7 +1770,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>224</v>
       </c>
@@ -1772,7 +1784,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>78</v>
       </c>
@@ -1786,7 +1798,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -1800,7 +1812,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>187</v>
       </c>
@@ -1814,7 +1826,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>325</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -1842,7 +1854,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>263</v>
       </c>
@@ -1856,7 +1868,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -1870,7 +1882,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -1884,7 +1896,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1898,7 +1910,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1912,7 +1924,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>205</v>
       </c>
@@ -1926,7 +1938,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>181</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>326</v>
       </c>
@@ -1954,7 +1966,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>208</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>212</v>
       </c>
@@ -1982,40 +1994,40 @@
         <v>259</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>346</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E32" t="s">
+        <v>203</v>
+      </c>
+      <c r="F32" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>204</v>
       </c>
-      <c r="F32" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="F33" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>226</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="E33" t="s">
-        <v>203</v>
-      </c>
-      <c r="F33" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>328</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="E34" t="s">
         <v>203</v>
@@ -2024,149 +2036,149 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>328</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E35" t="s">
+        <v>203</v>
+      </c>
+      <c r="F35" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>204</v>
       </c>
-      <c r="F35" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="F36" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E36" t="s">
-        <v>203</v>
-      </c>
-      <c r="F36" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="E37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F37" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>234</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F37" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="F38" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>330</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E38" t="s">
-        <v>203</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E39" t="s">
+        <v>203</v>
+      </c>
+      <c r="F39" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E39" t="s">
-        <v>203</v>
-      </c>
-      <c r="F39" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="E40" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E40" t="s">
-        <v>203</v>
-      </c>
-      <c r="F40" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="E41" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>236</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E41" t="s">
-        <v>203</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E42" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E42" t="s">
-        <v>203</v>
-      </c>
-      <c r="F42" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="E43" t="s">
+        <v>203</v>
+      </c>
+      <c r="F43" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E43" t="s">
-        <v>203</v>
-      </c>
-      <c r="F43" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="E44" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E44" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>102</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="E45" t="s">
         <v>203</v>
@@ -2175,12 +2187,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>175</v>
+        <v>103</v>
       </c>
       <c r="E46" t="s">
         <v>203</v>
@@ -2189,82 +2201,82 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" t="s">
+        <v>203</v>
+      </c>
+      <c r="F47" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>193</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E47" t="s">
-        <v>203</v>
-      </c>
-      <c r="F47" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="E48" t="s">
+        <v>203</v>
+      </c>
+      <c r="F48" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E48" t="s">
-        <v>203</v>
-      </c>
-      <c r="F48" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="E49" t="s">
+        <v>203</v>
+      </c>
+      <c r="F49" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E49" t="s">
-        <v>203</v>
-      </c>
-      <c r="F49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="E50" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>264</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E50" t="s">
-        <v>203</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E51" t="s">
+        <v>203</v>
+      </c>
+      <c r="F51" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>105</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E51" t="s">
-        <v>204</v>
-      </c>
-      <c r="F51" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>332</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="E52" t="s">
         <v>204</v>
@@ -2273,12 +2285,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>332</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>134</v>
+        <v>333</v>
       </c>
       <c r="E53" t="s">
         <v>204</v>
@@ -2287,12 +2299,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>334</v>
+        <v>133</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>335</v>
+        <v>134</v>
       </c>
       <c r="E54" t="s">
         <v>204</v>
@@ -2301,26 +2313,26 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>334</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E55" t="s">
-        <v>203</v>
-      </c>
-      <c r="F55" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E56" t="s">
         <v>203</v>
@@ -2329,40 +2341,40 @@
         <v>258</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" t="s">
+        <v>203</v>
+      </c>
+      <c r="F57" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>143</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E57" t="s">
-        <v>203</v>
-      </c>
-      <c r="F57" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="E58" t="s">
+        <v>203</v>
+      </c>
+      <c r="F58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E58" t="s">
-        <v>204</v>
-      </c>
-      <c r="F58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E59" t="s">
         <v>204</v>
@@ -2371,12 +2383,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>64</v>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>19</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="E60" t="s">
         <v>204</v>
@@ -2385,34 +2397,40 @@
         <v>259</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>344</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E61" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" t="s">
+        <v>204</v>
+      </c>
+      <c r="F62" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="E61" t="s">
-        <v>203</v>
-      </c>
-      <c r="F61" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>189</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E63" t="s">
         <v>203</v>
@@ -2421,54 +2439,48 @@
         <v>258</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E65" t="s">
+        <v>203</v>
+      </c>
+      <c r="F65" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>343</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E64" t="s">
-        <v>203</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E66" t="s">
+        <v>203</v>
+      </c>
+      <c r="F66" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>233</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="E65" t="s">
-        <v>204</v>
-      </c>
-      <c r="F65" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E66" t="s">
-        <v>203</v>
-      </c>
-      <c r="F66" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>219</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E67" t="s">
         <v>204</v>
@@ -2477,124 +2489,124 @@
         <v>259</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E68" t="s">
+        <v>203</v>
+      </c>
+      <c r="F68" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>219</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E69" t="s">
+        <v>204</v>
+      </c>
+      <c r="F69" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>260</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E68" t="s">
-        <v>203</v>
-      </c>
-      <c r="F68" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="E70" t="s">
+        <v>203</v>
+      </c>
+      <c r="F70" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>185</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E69" t="s">
-        <v>203</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E71" t="s">
+        <v>203</v>
+      </c>
+      <c r="F71" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>338</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E70" t="s">
-        <v>203</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E72" t="s">
+        <v>203</v>
+      </c>
+      <c r="F72" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>58</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E71" t="s">
-        <v>203</v>
-      </c>
-      <c r="F71" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="E73" t="s">
+        <v>203</v>
+      </c>
+      <c r="F73" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>191</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E72" t="s">
-        <v>203</v>
-      </c>
-      <c r="F72" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="E74" t="s">
+        <v>203</v>
+      </c>
+      <c r="F74" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>183</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E75" t="s">
         <v>204</v>
       </c>
-      <c r="F73" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="F75" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>32</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E74" t="s">
-        <v>204</v>
-      </c>
-      <c r="F74" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>179</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E75" t="s">
-        <v>203</v>
-      </c>
-      <c r="F75" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>17</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E76" t="s">
         <v>204</v>
@@ -2603,99 +2615,96 @@
         <v>259</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E77" t="s">
+        <v>203</v>
+      </c>
+      <c r="F77" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>204</v>
+      </c>
+      <c r="F78" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E79" t="s">
         <v>204</v>
       </c>
-      <c r="F77" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="F79" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E78" t="s">
-        <v>203</v>
-      </c>
-      <c r="F78" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="E80" t="s">
+        <v>203</v>
+      </c>
+      <c r="F80" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E79" t="s">
-        <v>203</v>
-      </c>
-      <c r="F79" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="E81" t="s">
+        <v>203</v>
+      </c>
+      <c r="F81" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E80" t="s">
-        <v>203</v>
-      </c>
-      <c r="F80" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="E82" t="s">
+        <v>203</v>
+      </c>
+      <c r="F82" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>129</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E81" t="s">
-        <v>204</v>
-      </c>
-      <c r="F81" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E82" t="s">
-        <v>204</v>
-      </c>
-      <c r="F82" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="E83" t="s">
         <v>204</v>
@@ -2704,12 +2713,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>210</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>108</v>
+        <v>211</v>
       </c>
       <c r="E84" t="s">
         <v>204</v>
@@ -2718,110 +2727,113 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>204</v>
+      </c>
+      <c r="F85" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E86" t="s">
+        <v>204</v>
+      </c>
+      <c r="F86" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>177</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E85" t="s">
-        <v>203</v>
-      </c>
-      <c r="F85" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="E87" t="s">
+        <v>203</v>
+      </c>
+      <c r="F87" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>123</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E86" t="s">
-        <v>203</v>
-      </c>
-      <c r="F86" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="E88" t="s">
+        <v>203</v>
+      </c>
+      <c r="F88" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E87" t="s">
-        <v>203</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E89" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E88" t="s">
-        <v>203</v>
-      </c>
-      <c r="F88" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="E90" t="s">
+        <v>203</v>
+      </c>
+      <c r="F90" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E89" t="s">
-        <v>203</v>
-      </c>
-      <c r="F89" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+      <c r="E91" t="s">
+        <v>203</v>
+      </c>
+      <c r="F91" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E90" t="s">
-        <v>204</v>
-      </c>
-      <c r="F90" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E91" t="s">
-        <v>204</v>
-      </c>
-      <c r="F91" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>43</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E92" t="s">
         <v>204</v>
@@ -2830,29 +2842,26 @@
         <v>259</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>195</v>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>196</v>
+        <v>44</v>
       </c>
       <c r="E93" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F93" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>41</v>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>43</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E94" t="s">
         <v>204</v>
@@ -2861,85 +2870,94 @@
         <v>259</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>195</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E95" t="s">
+        <v>203</v>
+      </c>
+      <c r="F95" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E96" t="s">
+        <v>204</v>
+      </c>
+      <c r="F96" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C95" s="1"/>
-      <c r="E95" t="s">
-        <v>203</v>
-      </c>
-      <c r="F95" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="C97" s="1"/>
+      <c r="E97" t="s">
+        <v>203</v>
+      </c>
+      <c r="F97" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>141</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E96" t="s">
-        <v>203</v>
-      </c>
-      <c r="F96" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="E98" t="s">
+        <v>203</v>
+      </c>
+      <c r="F98" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>38</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E99" t="s">
         <v>204</v>
       </c>
-      <c r="F97" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="F99" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>15</v>
       </c>
-      <c r="C98" t="s">
-        <v>0</v>
-      </c>
-      <c r="G98" s="2">
+      <c r="C100" t="s">
+        <v>0</v>
+      </c>
+      <c r="G100" s="2">
         <v>43221</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>14</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G99" s="2">
-        <v>43221</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>125</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I100" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>9</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>0</v>
@@ -2948,76 +2966,75 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>145</v>
-      </c>
-      <c r="C102" t="s">
+        <v>125</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I102" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G103" s="2">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>145</v>
+      </c>
+      <c r="C104" t="s">
+        <v>0</v>
+      </c>
+      <c r="I104" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>146</v>
       </c>
-      <c r="C103" t="s">
-        <v>0</v>
-      </c>
-      <c r="I103" s="2">
+      <c r="C105" t="s">
+        <v>0</v>
+      </c>
+      <c r="I105" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>7</v>
       </c>
-      <c r="C104" t="s">
-        <v>0</v>
-      </c>
-      <c r="H104" s="2">
+      <c r="C106" t="s">
+        <v>0</v>
+      </c>
+      <c r="H106" s="2">
         <v>43313</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>8</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G105" s="2">
+      <c r="C107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G107" s="2">
         <v>43221</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>147</v>
-      </c>
-      <c r="C106" t="s">
-        <v>0</v>
-      </c>
-      <c r="I106" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>237</v>
-      </c>
-      <c r="C107" t="s">
-        <v>0</v>
-      </c>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>148</v>
       </c>
       <c r="C108" t="s">
         <v>0</v>
@@ -3026,20 +3043,21 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="C109" t="s">
         <v>0</v>
       </c>
+      <c r="I109" s="2"/>
       <c r="J109" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C110" t="s">
         <v>0</v>
@@ -3048,225 +3066,224 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="C111" t="s">
         <v>0</v>
       </c>
-      <c r="I111" s="2"/>
       <c r="J111" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>149</v>
+      </c>
+      <c r="C112" t="s">
+        <v>0</v>
+      </c>
+      <c r="I112" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>238</v>
+      </c>
+      <c r="C113" t="s">
+        <v>0</v>
+      </c>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>239</v>
       </c>
-      <c r="C112" t="s">
-        <v>0</v>
-      </c>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2">
+      <c r="C114" t="s">
+        <v>0</v>
+      </c>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>150</v>
       </c>
-      <c r="C113" t="s">
-        <v>0</v>
-      </c>
-      <c r="I113" s="2">
+      <c r="C115" t="s">
+        <v>0</v>
+      </c>
+      <c r="I115" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G114" s="2">
+      <c r="C116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G116" s="2">
         <v>43221</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>240</v>
       </c>
-      <c r="C115" t="s">
-        <v>0</v>
-      </c>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>6</v>
-      </c>
-      <c r="C116" t="s">
-        <v>0</v>
-      </c>
-      <c r="H116" s="2">
-        <v>43313</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>6</v>
-      </c>
       <c r="C117" t="s">
         <v>0</v>
       </c>
+      <c r="I117" s="2"/>
       <c r="J117" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" t="s">
+        <v>0</v>
+      </c>
+      <c r="H118" s="2">
+        <v>43313</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" t="s">
+        <v>0</v>
+      </c>
+      <c r="J119" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>241</v>
       </c>
-      <c r="C118" t="s">
-        <v>0</v>
-      </c>
-      <c r="I118" s="2"/>
-      <c r="J118" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>151</v>
-      </c>
-      <c r="C119" t="s">
-        <v>0</v>
-      </c>
-      <c r="I119" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>217</v>
-      </c>
       <c r="C120" t="s">
         <v>0</v>
       </c>
+      <c r="I120" s="2"/>
       <c r="J120" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>11</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G121" s="2">
-        <v>43221</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="C121" t="s">
+        <v>0</v>
+      </c>
+      <c r="I121" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
       </c>
-      <c r="I122" s="2"/>
       <c r="J122" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>11</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G123" s="2">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>242</v>
+      </c>
+      <c r="C124" t="s">
+        <v>0</v>
+      </c>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>243</v>
       </c>
-      <c r="C123" t="s">
-        <v>0</v>
-      </c>
-      <c r="I123" s="2"/>
-      <c r="J123" s="2">
+      <c r="C125" t="s">
+        <v>0</v>
+      </c>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>152</v>
       </c>
-      <c r="C124" t="s">
-        <v>0</v>
-      </c>
-      <c r="I124" s="2">
+      <c r="C126" t="s">
+        <v>0</v>
+      </c>
+      <c r="I126" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>12</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G125" s="2">
+      <c r="C127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G127" s="2">
         <v>43221</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>3</v>
       </c>
-      <c r="C126" t="s">
-        <v>0</v>
-      </c>
-      <c r="H126" s="2">
+      <c r="C128" t="s">
+        <v>0</v>
+      </c>
+      <c r="H128" s="2">
         <v>43313</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>153</v>
       </c>
-      <c r="C127" t="s">
-        <v>0</v>
-      </c>
-      <c r="I127" s="2">
+      <c r="C129" t="s">
+        <v>0</v>
+      </c>
+      <c r="I129" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>244</v>
-      </c>
-      <c r="C128" t="s">
-        <v>0</v>
-      </c>
-      <c r="I128" s="2"/>
-      <c r="J128" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>218</v>
-      </c>
-      <c r="C129" t="s">
-        <v>0</v>
-      </c>
-      <c r="J129" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>245</v>
       </c>
       <c r="C130" t="s">
         <v>0</v>
@@ -3276,122 +3293,122 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="C131" t="s">
         <v>0</v>
       </c>
-      <c r="I131" s="2"/>
       <c r="J131" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
+        <v>245</v>
+      </c>
+      <c r="C132" t="s">
+        <v>0</v>
+      </c>
+      <c r="I132" s="2"/>
+      <c r="J132" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>246</v>
+      </c>
+      <c r="C133" t="s">
+        <v>0</v>
+      </c>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>154</v>
       </c>
-      <c r="C132" t="s">
-        <v>0</v>
-      </c>
-      <c r="I132" s="2">
+      <c r="C134" t="s">
+        <v>0</v>
+      </c>
+      <c r="I134" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>155</v>
       </c>
-      <c r="C133" t="s">
-        <v>0</v>
-      </c>
-      <c r="I133" s="2">
+      <c r="C135" t="s">
+        <v>0</v>
+      </c>
+      <c r="I135" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>247</v>
       </c>
-      <c r="C134" t="s">
-        <v>0</v>
-      </c>
-      <c r="I134" s="2"/>
-      <c r="J134" s="2">
+      <c r="C136" t="s">
+        <v>0</v>
+      </c>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>2</v>
       </c>
-      <c r="C135" t="s">
-        <v>0</v>
-      </c>
-      <c r="H135" s="2">
+      <c r="C137" t="s">
+        <v>0</v>
+      </c>
+      <c r="H137" s="2">
         <v>43313</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>156</v>
       </c>
-      <c r="C136" t="s">
-        <v>0</v>
-      </c>
-      <c r="I136" s="2">
+      <c r="C138" t="s">
+        <v>0</v>
+      </c>
+      <c r="I138" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>220</v>
       </c>
-      <c r="C137" t="s">
-        <v>0</v>
-      </c>
-      <c r="J137" s="2">
+      <c r="C139" t="s">
+        <v>0</v>
+      </c>
+      <c r="J139" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>221</v>
       </c>
-      <c r="C138" t="s">
-        <v>0</v>
-      </c>
-      <c r="J138" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>157</v>
-      </c>
-      <c r="C139" t="s">
-        <v>0</v>
-      </c>
-      <c r="I139" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>248</v>
-      </c>
       <c r="C140" t="s">
         <v>0</v>
       </c>
-      <c r="I140" s="2"/>
       <c r="J140" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C141" t="s">
         <v>0</v>
@@ -3400,125 +3417,125 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
+        <v>248</v>
+      </c>
+      <c r="C142" t="s">
+        <v>0</v>
+      </c>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>158</v>
+      </c>
+      <c r="C143" t="s">
+        <v>0</v>
+      </c>
+      <c r="I143" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>159</v>
       </c>
-      <c r="C142" t="s">
-        <v>0</v>
-      </c>
-      <c r="I142" s="2">
+      <c r="C144" t="s">
+        <v>0</v>
+      </c>
+      <c r="I144" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>249</v>
       </c>
-      <c r="C143" t="s">
-        <v>0</v>
-      </c>
-      <c r="I143" s="2"/>
-      <c r="J143" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>222</v>
-      </c>
-      <c r="C144" t="s">
-        <v>0</v>
-      </c>
-      <c r="J144" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>223</v>
-      </c>
       <c r="C145" t="s">
         <v>0</v>
       </c>
+      <c r="I145" s="2"/>
       <c r="J145" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>160</v>
+        <v>222</v>
       </c>
       <c r="C146" t="s">
         <v>0</v>
       </c>
-      <c r="I146" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J146" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="C147" t="s">
         <v>0</v>
       </c>
-      <c r="I147" s="2"/>
       <c r="J147" s="2">
         <v>43678</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="C148" t="s">
         <v>0</v>
-      </c>
-      <c r="H148" s="2">
-        <v>43313</v>
       </c>
       <c r="I148" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="C149" t="s">
         <v>0</v>
       </c>
-      <c r="I149" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I149" s="2"/>
+      <c r="J149" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>162</v>
+        <v>4</v>
       </c>
       <c r="C150" t="s">
         <v>0</v>
+      </c>
+      <c r="H150" s="2">
+        <v>43313</v>
       </c>
       <c r="I150" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>251</v>
+        <v>161</v>
       </c>
       <c r="C151" t="s">
         <v>0</v>
       </c>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I151" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C152" t="s">
         <v>0</v>
@@ -3527,20 +3544,21 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>164</v>
+        <v>251</v>
       </c>
       <c r="C153" t="s">
         <v>0</v>
       </c>
-      <c r="I153" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I153" s="2"/>
+      <c r="J153" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C154" t="s">
         <v>0</v>
@@ -3549,21 +3567,20 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>252</v>
+        <v>164</v>
       </c>
       <c r="C155" t="s">
         <v>0</v>
       </c>
-      <c r="I155" s="2"/>
-      <c r="J155" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I155" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C156" t="s">
         <v>0</v>
@@ -3572,54 +3589,54 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>252</v>
+      </c>
+      <c r="C157" t="s">
+        <v>0</v>
+      </c>
+      <c r="I157" s="2"/>
+      <c r="J157" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>166</v>
+      </c>
+      <c r="C158" t="s">
+        <v>0</v>
+      </c>
+      <c r="I158" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>5</v>
       </c>
-      <c r="C157" t="s">
-        <v>0</v>
-      </c>
-      <c r="H157" s="2">
+      <c r="C159" t="s">
+        <v>0</v>
+      </c>
+      <c r="H159" s="2">
         <v>43313</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>1</v>
       </c>
-      <c r="C158" t="s">
-        <v>0</v>
-      </c>
-      <c r="H158" s="2">
+      <c r="C160" t="s">
+        <v>0</v>
+      </c>
+      <c r="H160" s="2">
         <v>43313</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
         <v>110</v>
-      </c>
-      <c r="C159" t="s">
-        <v>0</v>
-      </c>
-      <c r="I159" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>253</v>
-      </c>
-      <c r="C160" t="s">
-        <v>0</v>
-      </c>
-      <c r="I160" s="2"/>
-      <c r="J160" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>167</v>
       </c>
       <c r="C161" t="s">
         <v>0</v>
@@ -3628,20 +3645,21 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>126</v>
+        <v>253</v>
       </c>
       <c r="C162" t="s">
         <v>0</v>
       </c>
-      <c r="I162" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I162" s="2"/>
+      <c r="J162" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="C163" t="s">
         <v>0</v>
@@ -3650,9 +3668,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>168</v>
+        <v>126</v>
       </c>
       <c r="C164" t="s">
         <v>0</v>
@@ -3661,9 +3679,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="C165" t="s">
         <v>0</v>
@@ -3672,9 +3690,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C166" t="s">
         <v>0</v>
@@ -3683,9 +3701,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C167" t="s">
         <v>0</v>
@@ -3694,23 +3712,20 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>13</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G168" s="2">
-        <v>43221</v>
+        <v>170</v>
+      </c>
+      <c r="C168" t="s">
+        <v>0</v>
       </c>
       <c r="I168" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="C169" t="s">
         <v>0</v>
@@ -3719,20 +3734,23 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>112</v>
-      </c>
-      <c r="C170" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G170" s="2">
+        <v>43221</v>
       </c>
       <c r="I170" s="2">
         <v>43617</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C171" t="s">
         <v>0</v>
@@ -3741,9 +3759,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C172" t="s">
         <v>0</v>
@@ -3752,9 +3770,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C173" t="s">
         <v>0</v>
@@ -3763,9 +3781,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C174" t="s">
         <v>0</v>
@@ -3774,9 +3792,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C175" t="s">
         <v>0</v>
@@ -3785,9 +3803,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C176" t="s">
         <v>0</v>
@@ -3796,9 +3814,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C177" t="s">
         <v>0</v>
@@ -3807,20 +3825,20 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
+        <v>118</v>
+      </c>
+      <c r="C178" t="s">
+        <v>0</v>
+      </c>
+      <c r="I178" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
         <v>119</v>
-      </c>
-      <c r="C178" t="s">
-        <v>0</v>
-      </c>
-      <c r="J178" s="2">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>120</v>
       </c>
       <c r="C179" t="s">
         <v>0</v>
@@ -3829,20 +3847,20 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C180" t="s">
         <v>0</v>
       </c>
-      <c r="I180" s="2">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J180" s="2">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C181" t="s">
         <v>0</v>
@@ -3851,9 +3869,9 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C182" t="s">
         <v>0</v>
@@ -3862,619 +3880,641 @@
         <v>43617</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
+        <v>122</v>
+      </c>
+      <c r="C183" t="s">
+        <v>0</v>
+      </c>
+      <c r="I183" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>132</v>
+      </c>
+      <c r="C184" t="s">
+        <v>0</v>
+      </c>
+      <c r="I184" s="2">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
         <v>266</v>
       </c>
-      <c r="C183" t="s">
-        <v>0</v>
-      </c>
-      <c r="K183" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="C185" t="s">
+        <v>0</v>
+      </c>
+      <c r="K185" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
         <v>267</v>
       </c>
-      <c r="C184" t="s">
-        <v>0</v>
-      </c>
-      <c r="K184" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="C186" t="s">
+        <v>0</v>
+      </c>
+      <c r="K186" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
         <v>268</v>
       </c>
-      <c r="C185" t="s">
-        <v>0</v>
-      </c>
-      <c r="K185" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="C187" t="s">
+        <v>0</v>
+      </c>
+      <c r="K187" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
         <v>269</v>
       </c>
-      <c r="C186" t="s">
-        <v>0</v>
-      </c>
-      <c r="K186" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="C188" t="s">
+        <v>0</v>
+      </c>
+      <c r="K188" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
         <v>270</v>
       </c>
-      <c r="C187" t="s">
-        <v>0</v>
-      </c>
-      <c r="K187" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="C189" t="s">
+        <v>0</v>
+      </c>
+      <c r="K189" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
         <v>271</v>
       </c>
-      <c r="C188" t="s">
-        <v>0</v>
-      </c>
-      <c r="K188" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="C190" t="s">
+        <v>0</v>
+      </c>
+      <c r="K190" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
         <v>272</v>
       </c>
-      <c r="C189" t="s">
-        <v>0</v>
-      </c>
-      <c r="K189" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="C191" t="s">
+        <v>0</v>
+      </c>
+      <c r="K191" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
         <v>273</v>
       </c>
-      <c r="C190" t="s">
-        <v>0</v>
-      </c>
-      <c r="K190" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="C192" t="s">
+        <v>0</v>
+      </c>
+      <c r="K192" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
         <v>274</v>
       </c>
-      <c r="C191" t="s">
-        <v>0</v>
-      </c>
-      <c r="K191" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="C193" t="s">
+        <v>0</v>
+      </c>
+      <c r="K193" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
         <v>275</v>
       </c>
-      <c r="C192" t="s">
-        <v>0</v>
-      </c>
-      <c r="K192" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="C194" t="s">
+        <v>0</v>
+      </c>
+      <c r="K194" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
         <v>276</v>
       </c>
-      <c r="C193" t="s">
-        <v>0</v>
-      </c>
-      <c r="K193" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="C195" t="s">
+        <v>0</v>
+      </c>
+      <c r="K195" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
         <v>277</v>
       </c>
-      <c r="C194" t="s">
-        <v>0</v>
-      </c>
-      <c r="K194" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="C196" t="s">
+        <v>0</v>
+      </c>
+      <c r="K196" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
         <v>278</v>
       </c>
-      <c r="C195" t="s">
-        <v>0</v>
-      </c>
-      <c r="K195" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="C197" t="s">
+        <v>0</v>
+      </c>
+      <c r="K197" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
         <v>279</v>
       </c>
-      <c r="C196" t="s">
-        <v>0</v>
-      </c>
-      <c r="K196" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="C198" t="s">
+        <v>0</v>
+      </c>
+      <c r="K198" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
         <v>280</v>
       </c>
-      <c r="C197" t="s">
-        <v>0</v>
-      </c>
-      <c r="K197" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="C199" t="s">
+        <v>0</v>
+      </c>
+      <c r="K199" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
         <v>281</v>
       </c>
-      <c r="C198" t="s">
-        <v>0</v>
-      </c>
-      <c r="K198" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="C200" t="s">
+        <v>0</v>
+      </c>
+      <c r="K200" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
         <v>282</v>
       </c>
-      <c r="C199" t="s">
-        <v>0</v>
-      </c>
-      <c r="K199" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="C201" t="s">
+        <v>0</v>
+      </c>
+      <c r="K201" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
         <v>283</v>
       </c>
-      <c r="C200" t="s">
-        <v>0</v>
-      </c>
-      <c r="K200" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="C202" t="s">
+        <v>0</v>
+      </c>
+      <c r="K202" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
         <v>284</v>
       </c>
-      <c r="C201" t="s">
-        <v>0</v>
-      </c>
-      <c r="K201" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="C203" t="s">
+        <v>0</v>
+      </c>
+      <c r="K203" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
         <v>285</v>
       </c>
-      <c r="C202" t="s">
-        <v>0</v>
-      </c>
-      <c r="K202" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="C204" t="s">
+        <v>0</v>
+      </c>
+      <c r="K204" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
         <v>286</v>
       </c>
-      <c r="C203" t="s">
-        <v>0</v>
-      </c>
-      <c r="K203" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="C205" t="s">
+        <v>0</v>
+      </c>
+      <c r="K205" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
         <v>287</v>
       </c>
-      <c r="C204" t="s">
-        <v>0</v>
-      </c>
-      <c r="K204" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="C206" t="s">
+        <v>0</v>
+      </c>
+      <c r="K206" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
         <v>288</v>
       </c>
-      <c r="C205" t="s">
-        <v>0</v>
-      </c>
-      <c r="K205" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="C207" t="s">
+        <v>0</v>
+      </c>
+      <c r="K207" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
         <v>289</v>
       </c>
-      <c r="C206" t="s">
-        <v>0</v>
-      </c>
-      <c r="K206" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="C208" t="s">
+        <v>0</v>
+      </c>
+      <c r="K208" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
         <v>290</v>
       </c>
-      <c r="C207" t="s">
-        <v>0</v>
-      </c>
-      <c r="K207" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="C209" t="s">
+        <v>0</v>
+      </c>
+      <c r="K209" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
         <v>291</v>
       </c>
-      <c r="C208" t="s">
-        <v>0</v>
-      </c>
-      <c r="K208" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="C210" t="s">
+        <v>0</v>
+      </c>
+      <c r="K210" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
         <v>292</v>
       </c>
-      <c r="C209" t="s">
-        <v>0</v>
-      </c>
-      <c r="K209" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="C211" t="s">
+        <v>0</v>
+      </c>
+      <c r="K211" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
         <v>293</v>
       </c>
-      <c r="C210" t="s">
-        <v>0</v>
-      </c>
-      <c r="K210" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="C212" t="s">
+        <v>0</v>
+      </c>
+      <c r="K212" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
         <v>294</v>
       </c>
-      <c r="C211" t="s">
-        <v>0</v>
-      </c>
-      <c r="K211" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="C213" t="s">
+        <v>0</v>
+      </c>
+      <c r="K213" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
         <v>295</v>
       </c>
-      <c r="C212" t="s">
-        <v>0</v>
-      </c>
-      <c r="K212" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="C214" t="s">
+        <v>0</v>
+      </c>
+      <c r="K214" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
         <v>296</v>
       </c>
-      <c r="C213" t="s">
-        <v>0</v>
-      </c>
-      <c r="K213" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="C215" t="s">
+        <v>0</v>
+      </c>
+      <c r="K215" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
         <v>297</v>
       </c>
-      <c r="C214" t="s">
-        <v>0</v>
-      </c>
-      <c r="K214" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="C216" t="s">
+        <v>0</v>
+      </c>
+      <c r="K216" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
         <v>298</v>
       </c>
-      <c r="C215" t="s">
-        <v>0</v>
-      </c>
-      <c r="K215" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="C217" t="s">
+        <v>0</v>
+      </c>
+      <c r="K217" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
         <v>299</v>
       </c>
-      <c r="C216" t="s">
-        <v>0</v>
-      </c>
-      <c r="K216" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="C218" t="s">
+        <v>0</v>
+      </c>
+      <c r="K218" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
         <v>300</v>
       </c>
-      <c r="C217" t="s">
-        <v>0</v>
-      </c>
-      <c r="K217" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="C219" t="s">
+        <v>0</v>
+      </c>
+      <c r="K219" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
         <v>301</v>
       </c>
-      <c r="C218" t="s">
-        <v>0</v>
-      </c>
-      <c r="K218" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="C220" t="s">
+        <v>0</v>
+      </c>
+      <c r="K220" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
         <v>302</v>
       </c>
-      <c r="C219" t="s">
-        <v>0</v>
-      </c>
-      <c r="K219" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="C221" t="s">
+        <v>0</v>
+      </c>
+      <c r="K221" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
         <v>303</v>
       </c>
-      <c r="C220" t="s">
-        <v>0</v>
-      </c>
-      <c r="K220" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="C222" t="s">
+        <v>0</v>
+      </c>
+      <c r="K222" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
         <v>304</v>
       </c>
-      <c r="C221" t="s">
-        <v>0</v>
-      </c>
-      <c r="K221" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+      <c r="C223" t="s">
+        <v>0</v>
+      </c>
+      <c r="K223" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
         <v>305</v>
       </c>
-      <c r="C222" t="s">
-        <v>0</v>
-      </c>
-      <c r="K222" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+      <c r="C224" t="s">
+        <v>0</v>
+      </c>
+      <c r="K224" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
         <v>306</v>
       </c>
-      <c r="C223" t="s">
-        <v>0</v>
-      </c>
-      <c r="K223" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+      <c r="C225" t="s">
+        <v>0</v>
+      </c>
+      <c r="K225" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
         <v>307</v>
       </c>
-      <c r="C224" t="s">
-        <v>0</v>
-      </c>
-      <c r="K224" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+      <c r="C226" t="s">
+        <v>0</v>
+      </c>
+      <c r="K226" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
         <v>308</v>
       </c>
-      <c r="C225" t="s">
-        <v>0</v>
-      </c>
-      <c r="K225" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
+      <c r="C227" t="s">
+        <v>0</v>
+      </c>
+      <c r="K227" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
         <v>309</v>
       </c>
-      <c r="C226" t="s">
-        <v>0</v>
-      </c>
-      <c r="K226" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+      <c r="C228" t="s">
+        <v>0</v>
+      </c>
+      <c r="K228" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
         <v>310</v>
       </c>
-      <c r="C227" t="s">
-        <v>0</v>
-      </c>
-      <c r="K227" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+      <c r="C229" t="s">
+        <v>0</v>
+      </c>
+      <c r="K229" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
         <v>311</v>
       </c>
-      <c r="C228" t="s">
-        <v>0</v>
-      </c>
-      <c r="K228" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
+      <c r="C230" t="s">
+        <v>0</v>
+      </c>
+      <c r="K230" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
         <v>312</v>
       </c>
-      <c r="C229" t="s">
-        <v>0</v>
-      </c>
-      <c r="K229" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
+      <c r="C231" t="s">
+        <v>0</v>
+      </c>
+      <c r="K231" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
         <v>313</v>
       </c>
-      <c r="C230" t="s">
-        <v>0</v>
-      </c>
-      <c r="K230" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
+      <c r="C232" t="s">
+        <v>0</v>
+      </c>
+      <c r="K232" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
         <v>314</v>
       </c>
-      <c r="C231" t="s">
-        <v>0</v>
-      </c>
-      <c r="K231" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
+      <c r="C233" t="s">
+        <v>0</v>
+      </c>
+      <c r="K233" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
         <v>315</v>
       </c>
-      <c r="C232" t="s">
-        <v>0</v>
-      </c>
-      <c r="K232" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+      <c r="C234" t="s">
+        <v>0</v>
+      </c>
+      <c r="K234" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
         <v>316</v>
       </c>
-      <c r="C233" t="s">
-        <v>0</v>
-      </c>
-      <c r="K233" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+      <c r="C235" t="s">
+        <v>0</v>
+      </c>
+      <c r="K235" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
         <v>317</v>
       </c>
-      <c r="C234" t="s">
-        <v>0</v>
-      </c>
-      <c r="K234" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
+      <c r="C236" t="s">
+        <v>0</v>
+      </c>
+      <c r="K236" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
         <v>318</v>
       </c>
-      <c r="C235" t="s">
-        <v>0</v>
-      </c>
-      <c r="K235" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
+      <c r="C237" t="s">
+        <v>0</v>
+      </c>
+      <c r="K237" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
         <v>319</v>
       </c>
-      <c r="C236" t="s">
-        <v>0</v>
-      </c>
-      <c r="K236" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+      <c r="C238" t="s">
+        <v>0</v>
+      </c>
+      <c r="K238" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
         <v>320</v>
       </c>
-      <c r="C237" t="s">
-        <v>0</v>
-      </c>
-      <c r="K237" s="7">
-        <v>44032</v>
-      </c>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
+      <c r="C239" t="s">
+        <v>0</v>
+      </c>
+      <c r="K239" s="7">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
         <v>321</v>
       </c>
-      <c r="C238" t="s">
-        <v>0</v>
-      </c>
-      <c r="K238" s="7">
+      <c r="C240" t="s">
+        <v>0</v>
+      </c>
+      <c r="K240" s="7">
         <v>44032</v>
       </c>
     </row>

</xml_diff>